<commit_message>
The project has updated
</commit_message>
<xml_diff>
--- a/src/test/java/apachePOI/resource/_ApachePOIWriteInTheExcel.xlsx
+++ b/src/test/java/apachePOI/resource/_ApachePOIWriteInTheExcel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
   <si>
     <t>Apache POI</t>
   </si>
@@ -968,7 +968,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -991,6 +991,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>